<commit_message>
skriptik pro konverzi csv->json
</commit_message>
<xml_diff>
--- a/data/diplomka_events_artworks_styles_1.xlsx
+++ b/data/diplomka_events_artworks_styles_1.xlsx
@@ -22,9 +22,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="149">
-  <si>
-    <t>jjjjjj</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="145">
+  <si>
+    <t>start</t>
   </si>
   <si>
     <t>end</t>
@@ -270,18 +270,12 @@
     <t>FAVU established</t>
   </si>
   <si>
-    <t>year</t>
-  </si>
-  <si>
     <t>first</t>
   </si>
   <si>
     <t>last</t>
   </si>
   <si>
-    <t>artwork</t>
-  </si>
-  <si>
     <t>Ivan</t>
   </si>
   <si>
@@ -412,12 +406,6 @@
   </si>
   <si>
     <t>artworks/Strizek.jpg</t>
-  </si>
-  <si>
-    <t>start</t>
-  </si>
-  <si>
-    <t>style</t>
   </si>
   <si>
     <t>Imaginative art</t>
@@ -573,16 +561,16 @@
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.6814814814815"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="40.137037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.25925925925926"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.4037037037037"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="42.137037037037"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.54444444444444"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="20.3814814814815"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.2703703703704"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1298,35 +1286,39 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="10.6814814814815"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1703703703704"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3259259259259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.8888888888889"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.27037037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="16.9518518518519"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.9148148148148"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.4555555555556"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.2703703703704"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>83</v>
       </c>
-      <c r="C1" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>85</v>
-      </c>
       <c r="E1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="0" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1334,201 +1326,201 @@
       <c r="A2" s="0" t="n">
         <v>1980</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="C2" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" s="0" t="s">
         <v>86</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>1981</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="C3" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="F3" s="0" t="s">
         <v>90</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <v>1983</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="F4" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
         <v>1983</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="C5" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="F5" s="0" t="s">
         <v>97</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
         <v>1984</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="C6" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="E6" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="F6" s="0" t="s">
         <v>101</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
         <v>1986</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="C7" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="F7" s="0" t="s">
         <v>104</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
         <v>1986</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="C8" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="F8" s="0" t="s">
         <v>108</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>109</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <v>1987</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="C9" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9" s="0" t="s">
         <v>111</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="F9" s="0" t="s">
         <v>112</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <v>1987</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="C10" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="F10" s="0" t="s">
         <v>116</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>117</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <v>1988</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="C11" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="E11" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="F11" s="0" t="s">
         <v>120</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <v>1989</v>
       </c>
-      <c r="B12" s="0" t="s">
-        <v>107</v>
-      </c>
       <c r="C12" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="F12" s="0" t="s">
         <v>123</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <v>1989</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="C13" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="E13" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="F13" s="0" t="s">
         <v>127</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1550,25 +1542,25 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.6814814814815"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="28.4185185185185"/>
-    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="29.7888888888889"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="11.2703703703704"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>131</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1579,7 +1571,7 @@
         <v>1995</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1590,7 +1582,7 @@
         <v>1970</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1601,7 +1593,7 @@
         <v>1975</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1612,7 +1604,7 @@
         <v>1960</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1623,7 +1615,7 @@
         <v>1980</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1634,7 +1626,7 @@
         <v>1955</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1645,7 +1637,7 @@
         <v>1995</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1656,7 +1648,7 @@
         <v>1965</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1667,7 +1659,7 @@
         <v>1955</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1678,7 +1670,7 @@
         <v>1965</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1689,7 +1681,7 @@
         <v>1967</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1700,7 +1692,7 @@
         <v>1985</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1711,7 +1703,7 @@
         <v>1985</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1722,7 +1714,7 @@
         <v>1965</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1733,7 +1725,7 @@
         <v>1987</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1744,7 +1736,7 @@
         <v>1995</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1755,7 +1747,7 @@
         <v>1993</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1766,7 +1758,7 @@
         <v>1995</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>